<commit_message>
Update Excel file report
</commit_message>
<xml_diff>
--- a/Docs/SIMS/sen0257UNO-ESP32calib_sim.xlsx
+++ b/Docs/SIMS/sen0257UNO-ESP32calib_sim.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Nabil\CodeCpp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Nabil\CodeCpp\Docs\SIMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sen0257UNOcalib_save" sheetId="1" r:id="rId1"/>
     <sheet name="Tension" sheetId="2" r:id="rId2"/>
     <sheet name="Pression" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -136,7 +136,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -617,7 +617,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -690,43 +690,1547 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>UNO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>sen0257UNOcalib_save!$D$2:$D$501</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="500"/>
+                <c:pt idx="0">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B55-4A35-9F91-141E28A52B47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -2272,1552 +3776,7 @@
         <c:smooth val="0"/>
         <c:axId val="292142880"/>
         <c:axId val="292142464"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>UNO</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>sen0257UNOcalib_save!$D$2:$D$501</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="500"/>
-                      <c:pt idx="0">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="100">
-                        <c:v>0.498</c:v>
-                      </c:pt>
-                      <c:pt idx="101">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="102">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="103">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="104">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="105">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="106">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="107">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="108">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="109">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="110">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="111">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="112">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="113">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="114">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="115">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="116">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="117">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="118">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="119">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="120">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="121">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="122">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="123">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="124">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="125">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="126">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="127">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="128">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="129">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="130">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="131">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="132">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="133">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="134">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="135">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="136">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="137">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="138">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="139">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="140">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="141">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="142">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="143">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="144">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="145">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="146">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="147">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="148">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="149">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="150">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="151">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="152">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="153">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="154">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="155">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="156">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="157">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="158">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="159">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="160">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="161">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="162">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="163">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="164">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="165">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="166">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="167">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="168">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="169">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="170">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="171">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="172">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="173">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="174">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="175">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="176">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="177">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="178">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="179">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="180">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="181">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="182">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="183">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="184">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="185">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="186">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="187">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="188">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="189">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="190">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="191">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="192">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="193">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="194">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="195">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="196">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="197">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="198">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="199">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="200">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="201">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="202">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="203">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="204">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="205">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="206">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="207">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="208">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="209">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="210">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="211">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="212">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="213">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="214">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="215">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="216">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="217">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="218">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="219">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="220">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="221">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="222">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="223">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="224">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="225">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="226">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="227">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="228">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="229">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="230">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="231">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="232">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="233">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="234">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="235">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="236">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="237">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="238">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="239">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="240">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="241">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="242">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="243">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="244">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="245">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="246">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="247">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="248">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="249">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="250">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="251">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="252">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="253">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="254">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="255">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="256">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="257">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="258">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="259">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="260">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="261">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="262">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="263">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="264">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="265">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="266">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="267">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="268">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="269">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="270">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="271">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="272">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="273">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="274">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="275">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="276">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="277">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="278">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="279">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="280">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="281">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="282">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="283">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="284">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="285">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="286">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="287">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="288">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="289">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="290">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="291">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="292">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="293">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="294">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="295">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="296">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="297">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="298">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="299">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="300">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="301">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="302">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="303">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="304">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="305">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="306">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="307">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="308">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="309">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="310">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="311">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="312">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="313">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="314">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="315">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="316">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="317">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="318">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="319">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="320">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="321">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="322">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="323">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="324">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="325">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="326">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="327">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="328">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="329">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="330">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="331">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="332">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="333">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="334">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="335">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="336">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="337">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="338">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="339">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="340">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="341">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="342">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="343">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="344">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="345">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="346">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="347">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="348">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="349">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="350">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="351">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="352">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="353">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="354">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="355">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="356">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="357">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="358">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="359">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="360">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="361">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="362">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="363">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="364">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="365">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="366">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="367">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="368">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="369">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="370">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="371">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="372">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="373">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="374">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="375">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="376">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="377">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="378">
-                        <c:v>0.498</c:v>
-                      </c:pt>
-                      <c:pt idx="379">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="380">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="381">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="382">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="383">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="384">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="385">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="386">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="387">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="388">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="389">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="390">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="391">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="392">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="393">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="394">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="395">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="396">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="397">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="398">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="399">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="400">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="401">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="402">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="403">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="404">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="405">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="406">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="407">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="408">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="409">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="410">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="411">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="412">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="413">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="414">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="415">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="416">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="417">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="418">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="419">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="420">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="421">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="422">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="423">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="424">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="425">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="426">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="427">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="428">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="429">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="430">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="431">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="432">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="433">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="434">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="435">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="436">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="437">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="438">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="439">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="440">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="441">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="442">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="443">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="444">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="445">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="446">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="447">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="448">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="449">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="450">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="451">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="452">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="453">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="454">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="455">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="456">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="457">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="458">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="459">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="460">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="461">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="462">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="463">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="464">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="465">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="466">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="467">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="468">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="469">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="470">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="471">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="472">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="473">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="474">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="475">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="476">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="477">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="478">
-                        <c:v>0.49299999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="479">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="480">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="481">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="482">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="483">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="484">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="485">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="486">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="487">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="488">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="489">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="490">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="491">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="492">
-                        <c:v>0.47899999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="493">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="494">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="495">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="496">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="497">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="498">
-                        <c:v>0.48799999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="499">
-                        <c:v>0.48299999999999998</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-5B55-4A35-9F91-141E28A52B47}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="292142880"/>
@@ -8703,7 +8662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1744"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
@@ -44830,7 +44789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>